<commit_message>
Added extend Report functionality
</commit_message>
<xml_diff>
--- a/ApiResponceComp/Files/File1.xlsx
+++ b/ApiResponceComp/Files/File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b0097042/git/apiJSONResponceComparison/ApiResponceComp/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DD40EAC-EF3C-6A42-994F-57071EC34DC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48693D48-B4B2-0F49-B193-4C7158035E88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{8F06B00B-5419-014D-A00B-3618D6FFAAA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>https://reqres.in/api/users/3</t>
   </si>
@@ -43,10 +43,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +77,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,7 +402,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,9 +416,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Update Test Data files
</commit_message>
<xml_diff>
--- a/ApiResponceComp/Files/File1.xlsx
+++ b/ApiResponceComp/Files/File1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b0097042/git/apiJSONResponceComparison/ApiResponceComp/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48693D48-B4B2-0F49-B193-4C7158035E88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D8C3D6-7934-8F41-AFE1-C2994D854C00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{8F06B00B-5419-014D-A00B-3618D6FFAAA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
   <si>
     <t>https://reqres.in/api/users/3</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09638E0-3381-CE4C-9F29-C17E4B3E0D37}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A17" sqref="A17:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,6 +448,66 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>